<commit_message>
Updated LOC and SD job for creation processing
</commit_message>
<xml_diff>
--- a/FedExCILOrderCreationProcess/src/main/resources/FedExCILTestResult_STG.xlsx
+++ b/FedExCILOrderCreationProcess/src/main/resources/FedExCILTestResult_STG.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
   <si>
     <t>FileName</t>
   </si>
@@ -28,12 +28,6 @@
     <t>FDXLoadTndr_1272020_206_19663458</t>
   </si>
   <si>
-    <t>FDXLoadTndr_1272020_206_19663460</t>
-  </si>
-  <si>
-    <t>FDXLoadTndr_1272020_216_19663511</t>
-  </si>
-  <si>
     <t>FDXLoadTndr_1272020_1918_19663362</t>
   </si>
   <si>
@@ -67,214 +61,73 @@
     <t>FDXLoadTndr_1282020_189_19667476</t>
   </si>
   <si>
-    <t>32483151</t>
-  </si>
-  <si>
-    <t>32483152</t>
-  </si>
-  <si>
-    <t>32483153</t>
-  </si>
-  <si>
-    <t>32483154</t>
-  </si>
-  <si>
-    <t>32483155</t>
-  </si>
-  <si>
-    <t>32483156</t>
-  </si>
-  <si>
-    <t>32483157</t>
-  </si>
-  <si>
-    <t>32483158</t>
-  </si>
-  <si>
-    <t>32483159</t>
-  </si>
-  <si>
-    <t>32483160</t>
-  </si>
-  <si>
-    <t>32584536</t>
-  </si>
-  <si>
-    <t>32584537</t>
-  </si>
-  <si>
-    <t>32584538</t>
-  </si>
-  <si>
-    <t>32584539</t>
-  </si>
-  <si>
-    <t>32584540</t>
-  </si>
-  <si>
-    <t>32584541</t>
-  </si>
-  <si>
-    <t>32584542</t>
-  </si>
-  <si>
-    <t>32584543</t>
-  </si>
-  <si>
-    <t>32584544</t>
-  </si>
-  <si>
-    <t>32584545</t>
-  </si>
-  <si>
-    <t>32584546</t>
-  </si>
-  <si>
-    <t>32584547</t>
-  </si>
-  <si>
-    <t>32584548</t>
-  </si>
-  <si>
-    <t>32584549</t>
-  </si>
-  <si>
-    <t>32584550</t>
-  </si>
-  <si>
-    <t>32584555</t>
-  </si>
-  <si>
-    <t>32584556</t>
-  </si>
-  <si>
-    <t>32584557</t>
-  </si>
-  <si>
-    <t>32584558</t>
-  </si>
-  <si>
-    <t>32584559</t>
-  </si>
-  <si>
-    <t>32584561</t>
-  </si>
-  <si>
-    <t>32584562</t>
-  </si>
-  <si>
-    <t>32584563</t>
-  </si>
-  <si>
-    <t>32584564</t>
-  </si>
-  <si>
-    <t>32584565</t>
-  </si>
-  <si>
-    <t>32584566</t>
-  </si>
-  <si>
-    <t>32584567</t>
-  </si>
-  <si>
-    <t>32584568</t>
-  </si>
-  <si>
-    <t>32584569</t>
-  </si>
-  <si>
-    <t>32584571</t>
-  </si>
-  <si>
-    <t>32584575</t>
-  </si>
-  <si>
-    <t>32584576</t>
-  </si>
-  <si>
-    <t>32584577</t>
-  </si>
-  <si>
-    <t>32584578</t>
-  </si>
-  <si>
-    <t>32584579</t>
-  </si>
-  <si>
-    <t>32584580</t>
-  </si>
-  <si>
-    <t>32584581</t>
-  </si>
-  <si>
-    <t>32584582</t>
-  </si>
-  <si>
-    <t>32584584</t>
-  </si>
-  <si>
-    <t>32584585</t>
-  </si>
-  <si>
-    <t>32584586</t>
-  </si>
-  <si>
-    <t>32584587</t>
-  </si>
-  <si>
-    <t>32584588</t>
-  </si>
-  <si>
-    <t>32584589</t>
-  </si>
-  <si>
-    <t>32584590</t>
-  </si>
-  <si>
-    <t>32584592</t>
-  </si>
-  <si>
-    <t>32584593</t>
-  </si>
-  <si>
-    <t>32584594</t>
-  </si>
-  <si>
-    <t>32584595</t>
-  </si>
-  <si>
-    <t>32584596</t>
-  </si>
-  <si>
-    <t>32584597</t>
-  </si>
-  <si>
-    <t>32584598</t>
-  </si>
-  <si>
-    <t>32584599</t>
-  </si>
-  <si>
-    <t>32584600</t>
-  </si>
-  <si>
-    <t>32584601</t>
-  </si>
-  <si>
-    <t>32584603</t>
-  </si>
-  <si>
-    <t>32584604</t>
-  </si>
-  <si>
-    <t>32584605</t>
-  </si>
-  <si>
-    <t>32584606</t>
-  </si>
-  <si>
-    <t>32584607</t>
+    <t>FDXLoadTndr_822022_412_22834483</t>
+  </si>
+  <si>
+    <t>32589994</t>
+  </si>
+  <si>
+    <t>32589995</t>
+  </si>
+  <si>
+    <t>32589996</t>
+  </si>
+  <si>
+    <t>32589997</t>
+  </si>
+  <si>
+    <t>32589998</t>
+  </si>
+  <si>
+    <t>32589999</t>
+  </si>
+  <si>
+    <t>32590000</t>
+  </si>
+  <si>
+    <t>32590001</t>
+  </si>
+  <si>
+    <t>32590002</t>
+  </si>
+  <si>
+    <t>32590003</t>
+  </si>
+  <si>
+    <t>32590005</t>
+  </si>
+  <si>
+    <t>32590006</t>
+  </si>
+  <si>
+    <t>32590007</t>
+  </si>
+  <si>
+    <t>32590008</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>H3P</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>LOC</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>32590233</t>
+  </si>
+  <si>
+    <t>32590236</t>
   </si>
 </sst>
 </file>
@@ -282,10 +135,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -323,9 +182,16 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -627,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:AG15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -639,135 +505,159 @@
     <col min="2" max="2" customWidth="true" width="24.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="B2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>37</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>86</v>
-      </c>
+      <c r="B15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="3"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes of LOC and SD service processing done
</commit_message>
<xml_diff>
--- a/FedExCILOrderCreationProcess/src/main/resources/FedExCILTestResult_STG.xlsx
+++ b/FedExCILOrderCreationProcess/src/main/resources/FedExCILTestResult_STG.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="87">
   <si>
     <t>FileName</t>
   </si>
@@ -128,6 +128,153 @@
   </si>
   <si>
     <t>32590236</t>
+  </si>
+  <si>
+    <t>32590282</t>
+  </si>
+  <si>
+    <t>32599195</t>
+  </si>
+  <si>
+    <t>32948247</t>
+  </si>
+  <si>
+    <t>32948248</t>
+  </si>
+  <si>
+    <t>32963170</t>
+  </si>
+  <si>
+    <t>32963174</t>
+  </si>
+  <si>
+    <t>32963177</t>
+  </si>
+  <si>
+    <t>$0.00</t>
+  </si>
+  <si>
+    <t>32963179</t>
+  </si>
+  <si>
+    <t>32963225</t>
+  </si>
+  <si>
+    <t>32963282</t>
+  </si>
+  <si>
+    <t>32963374</t>
+  </si>
+  <si>
+    <t>32963449</t>
+  </si>
+  <si>
+    <t>32963459</t>
+  </si>
+  <si>
+    <t>32963491</t>
+  </si>
+  <si>
+    <t>32963504</t>
+  </si>
+  <si>
+    <t>32963564</t>
+  </si>
+  <si>
+    <t>32963578</t>
+  </si>
+  <si>
+    <t>32963634</t>
+  </si>
+  <si>
+    <t>32963748</t>
+  </si>
+  <si>
+    <t>32963800</t>
+  </si>
+  <si>
+    <t>32963975</t>
+  </si>
+  <si>
+    <t>32964066</t>
+  </si>
+  <si>
+    <t>32964082</t>
+  </si>
+  <si>
+    <t>32964113</t>
+  </si>
+  <si>
+    <t>32964148</t>
+  </si>
+  <si>
+    <t>32964156</t>
+  </si>
+  <si>
+    <t>32964177</t>
+  </si>
+  <si>
+    <t>32964190</t>
+  </si>
+  <si>
+    <t>32964423</t>
+  </si>
+  <si>
+    <t>32964439</t>
+  </si>
+  <si>
+    <t>32964456</t>
+  </si>
+  <si>
+    <t>32964468</t>
+  </si>
+  <si>
+    <t>32964493</t>
+  </si>
+  <si>
+    <t>32964503</t>
+  </si>
+  <si>
+    <t>32964516</t>
+  </si>
+  <si>
+    <t>32964525</t>
+  </si>
+  <si>
+    <t>32964543</t>
+  </si>
+  <si>
+    <t>32964567</t>
+  </si>
+  <si>
+    <t>32964612</t>
+  </si>
+  <si>
+    <t>32966017</t>
+  </si>
+  <si>
+    <t>32966024</t>
+  </si>
+  <si>
+    <t>32966035</t>
+  </si>
+  <si>
+    <t>32966049</t>
+  </si>
+  <si>
+    <t>32966078</t>
+  </si>
+  <si>
+    <t>32966094</t>
+  </si>
+  <si>
+    <t>32966492</t>
+  </si>
+  <si>
+    <t>32966495</t>
+  </si>
+  <si>
+    <t>32966504</t>
   </si>
 </sst>
 </file>
@@ -520,8 +667,8 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>16</v>
+      <c r="B2" t="s">
+        <v>42</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>31</v>
@@ -546,21 +693,21 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>33</v>
       </c>
       <c r="AF4" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>19</v>
+      <c r="B5" t="s">
+        <v>43</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>34</v>

</xml_diff>